<commit_message>
Builder handles money manager now
</commit_message>
<xml_diff>
--- a/Assets/Docs/Requirements Checklist aw.xlsx
+++ b/Assets/Docs/Requirements Checklist aw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Term 2\Software Architecture\Tower-DefenceV2\Assets\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5272CF49-7D05-4E9F-8F69-01BCDFB55FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19962EC1-5266-4F13-B4A5-3CD13FCFC262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{DFC97FD2-4022-1548-A7B7-2F9FA8F56567}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>Priority</t>
   </si>
@@ -204,40 +204,43 @@
     <t>• Enemies follow a non-straight path to the end goal.</t>
   </si>
   <si>
-    <t>When money balance changes, MoneyManager checks if building options from Builder class can be afforded. The BuyEnabler component (attached to BuyMenu UI object) observes MoneyManager and disables/enables buttons corresponding to a given tower, when onMoneyChanged event is triggered. Upgrades not yet possible.</t>
-  </si>
-  <si>
-    <t>When OnClick event is triggered in Cursor component, Builder class recieves clickInfo, from which it can check if the clicked Cell isFree.</t>
-  </si>
-  <si>
-    <t>Observer Pattern =&gt; for now only Builder class reacts to the onClick event, but I may decide to add SFX and VFX or something else later =&gt; coupling reduction.</t>
-  </si>
-  <si>
     <t>The list of avaiable towers can be adjusted in editor (Builder component). But to make them accessible, a button has to be added manually. (Likewise with removing / replacing towers)</t>
   </si>
   <si>
     <t>You can find all tower levels in each tower's prefab under TowerSlot.</t>
   </si>
   <si>
-    <t>GridXZ&lt;Cell&gt; is the class used for the grid. GridManager creates the grid. LevelSetUp determines which cells are marked as build zones, by detecting where the path tiles are placed and modifying neighbouring cells. (Cell.BuildZone = true). Builder class is observing Cursor class - when Cursor's onClick event is triggered, Builder reciever clickInfo containing information about the clicked Cell (clickedInfo). It then checks if the Cell is a buildzone and proceeds accordingly. If the tower is built or sold, Builder triggers an onBuilt or onSold event (TransactionData). MoneyManager observes Builder and adjusts money balance when the events are triggered.</t>
-  </si>
-  <si>
-    <t>Observer Pattern =&gt; for now only MoneyManager reacts to the onBuilt and onSold events, but I may decided to add SFX and VFX or something else later. =&gt; coupling reduction. (see below for why Builder observes Cursor)</t>
-  </si>
-  <si>
     <t>towers have no function or script for now, but have different visuals</t>
   </si>
   <si>
     <t>MoneyDisplay observes MoneyManager and adjusts the value shown when onMoneyChanged event is triggered.</t>
   </si>
   <si>
-    <t>Observer pattern =&gt; multiple components react to the onMoneyChanged event. Reduces coupling. MoneyManager unaffected if I modify how I enable purchases.</t>
-  </si>
-  <si>
     <t>Observer pattern =&gt; multiple components react to the onMoneyChanged event. Reduces coupling. MoneyManager unaffected if I change the display.</t>
   </si>
   <si>
-    <t>The Cursor's model changes colour based on if it's hovering over a Cell that returns CanBuild() as true or false (blue = true, red = false). There are placeholder indicators for the build and non build area.</t>
+    <t>GridXZ&lt;Cell&gt; is the class used for the grid. GridManager creates the grid. LevelSetUp determines which cells are marked as build zones, by detecting where the path tiles are placed and modifying neighbouring cells. (Cell.BuildZone = true). Builder is responsible for handling building/selling towers (including dealing with money balance). It obvserves the Cursor class and when onClick event is triggered, it builds/sells tower if possible, then subtracts/adds money to the balance.</t>
+  </si>
+  <si>
+    <t>When OnClick event is triggered in Cursor component, Builder component recieves clickInfo, from which it can check if the clicked Cell isFree.</t>
+  </si>
+  <si>
+    <t>Observer pattern, same as in row 17.</t>
+  </si>
+  <si>
+    <t>Observer Pattern =&gt; for now only Builder class reacts to the onClick event, but I may decide to add SFX and VFX or something else later =&gt; coupling reduction. I've already changed how money is managed, and I am glad to not had to remove any code from cursor for that.</t>
+  </si>
+  <si>
+    <t>When money balance changes, Builder class checks if building options from can be afforded. The BuyEnabler component (attached to BuyMenu UI object) observes Builder and disables/enables buttons corresponding to a given tower, when onMoneyChanged event is triggered. Upgrades not yet possible.</t>
+  </si>
+  <si>
+    <t>The Cursor's model changes colour based on if it's hovering over a Cell that returns CanBuild() as true or false (blue = true, red = false). There are placeholder indicators for the build and non build area =&gt; (color coded, reed = invalid, green valid)</t>
+  </si>
+  <si>
+    <t>The UI scales with screen size and the elements are anchored to edges of the screen, ensuring their correct location no matter the resolution.</t>
+  </si>
+  <si>
+    <t>Observer pattern =&gt; multiple components react to the onMoneyChanged event =&gt; more may come later. No need to add more variables to Builder class if SFX/VFX/something else is added later.</t>
   </si>
 </sst>
 </file>
@@ -740,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4204571-75E2-6C43-842D-3E9152E2A192}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -912,7 +915,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -922,7 +925,7 @@
         <v>56</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -936,17 +939,17 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="14"/>
       <c r="D19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -957,7 +960,7 @@
       <c r="B20" s="5"/>
       <c r="C20" s="15"/>
       <c r="D20" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1009,7 +1012,7 @@
       <c r="B25" s="5"/>
       <c r="C25" s="14"/>
       <c r="D25" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1024,17 +1027,17 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="15"/>
       <c r="D27" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -1055,7 +1058,7 @@
       <c r="B29" s="5"/>
       <c r="C29" s="14"/>
       <c r="D29" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1087,10 +1090,10 @@
       <c r="B33" s="5"/>
       <c r="C33" s="14"/>
       <c r="D33" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -1104,14 +1107,14 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="5"/>
-      <c r="C35" s="15"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1146,20 +1149,22 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="3"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
+      <c r="C40"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>

</xml_diff>

<commit_message>
one wave gets spawned
</commit_message>
<xml_diff>
--- a/Assets/Docs/Requirements Checklist aw.xlsx
+++ b/Assets/Docs/Requirements Checklist aw.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Term 2\Software Architecture\Tower-DefenceV2\Assets\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Term 2\Software Architecture\Tower-DefenceV2\Assets\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AA9528-30E4-483E-ACD3-5949B55A7E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCB30A5-B620-4C2E-9B41-035B2A59FD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{DFC97FD2-4022-1548-A7B7-2F9FA8F56567}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFC97FD2-4022-1548-A7B7-2F9FA8F56567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>Priority</t>
   </si>
@@ -261,13 +261,28 @@
     <t>Strategy pattern. I first implemented a test class, and it will be easier to replace it with a more complex class that also inherits from the same interface later on. I may also use different classes for spawning different sorts of enemies.</t>
   </si>
   <si>
-    <t>Enemies use navmesh to navigate to the goal. The enemies follow a set of navpoints along the path. They automatically find objects tagged as NavPoint and  save the coordinates to a navigation queue.</t>
-  </si>
-  <si>
     <t>Enemy visual assets are in game.</t>
   </si>
   <si>
     <t>TimerToWave observes the BuilderState and updates the display every time it recieves onTick event.</t>
+  </si>
+  <si>
+    <t>You can add Waves to a list in WaveSpawnerQueue (IWaveSpawnerStrategy). Waves contain a list of Batches. Batches contain adjustable enemy queues (List&lt;EnemySO&gt;) and adjustable intervals between each enemy spawned, as well as adjustable intervals between this and the next batch. SpawnEnemyFromSO (IEnemySpawnStrategy) spawns enemies from the Batch. Separating waves into batches lets one easily set non uniform intervals between enemies if that's desired. A single batch in a wave will also function with no issue, if the interval is supposed to be constant.</t>
+  </si>
+  <si>
+    <t>Strategy Pattern. Makes it easy to switch Wave/Enemy spawn methods. I.e. if the decision is made to change the enemy spawn method to one based on percentage chance of spawning a type of enemy.</t>
+  </si>
+  <si>
+    <t>Waves are stored in WaveManager object. Only wave 0 will be launched for now.</t>
+  </si>
+  <si>
+    <t>Enemies use navmesh to navigate to the goal. The enemies follow a set of navpoints along the path. They automatically find objects tagged as NavPoint and  save the coordinates to a navigation queue. They ignore collisions with each other.</t>
+  </si>
+  <si>
+    <t>IEnemy contains methods for setting these properties. The BasicEnemy (the only enemy class for now) inherits from this interface and these values are set when the object is spawned via IEnemySpawnStrategy</t>
+  </si>
+  <si>
+    <t>The properties are dictated via EnemySO scriptable objects, which should contain a component inheriting from Ienemy interface. Visuals adjustement is not yet possible witout hard coding.</t>
   </si>
 </sst>
 </file>
@@ -770,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4204571-75E2-6C43-842D-3E9152E2A192}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -779,7 +794,8 @@
     <col min="1" max="1" width="118.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="33.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="47.125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
@@ -814,24 +830,30 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="189" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="236.25" x14ac:dyDescent="0.25">
@@ -880,14 +902,14 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="14"/>
       <c r="D9" s="3" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -902,13 +924,15 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
@@ -919,7 +943,7 @@
       <c r="B12" s="5"/>
       <c r="C12" s="15"/>
       <c r="D12" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -934,13 +958,15 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
@@ -1143,7 +1169,7 @@
       <c r="B34" s="5"/>
       <c r="C34" s="14"/>
       <c r="D34" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>

</xml_diff>